<commit_message>
django_backend Bugfix and changes.
</commit_message>
<xml_diff>
--- a/django_backend/var/sys/screen-template/template-v2.xlsx
+++ b/django_backend/var/sys/screen-template/template-v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-1005" yWindow="-105" windowWidth="29040" windowHeight="4170"/>
@@ -351,8 +351,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,7 +739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -786,17 +786,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -928,22 +917,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -971,7 +960,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -998,9 +987,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1019,7 +1005,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1093,6 +1079,11 @@
       <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1116,7 +1107,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1128,7 +1119,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1148,7 +1139,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1237,6 +1228,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1271,6 +1263,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1446,15 +1439,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -1480,7 +1471,7 @@
     <col min="28" max="30" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="37.5">
+    <row r="1" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1504,7 +1495,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1524,14 +1515,14 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1548,14 +1539,14 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="4"/>
@@ -1572,14 +1563,14 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="4"/>
@@ -1596,14 +1587,14 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
@@ -1622,14 +1613,14 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="12" t="s">
         <v>39</v>
       </c>
@@ -1648,14 +1639,14 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="4"/>
@@ -1672,14 +1663,14 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="12" t="s">
         <v>41</v>
       </c>
@@ -1698,14 +1689,14 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="4"/>
@@ -1722,14 +1713,14 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="12" t="s">
         <v>5</v>
       </c>
@@ -1748,14 +1739,14 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="12" t="s">
         <v>67</v>
       </c>
@@ -1774,14 +1765,14 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="12" t="s">
         <v>82</v>
       </c>
@@ -1800,14 +1791,14 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="4"/>
@@ -1824,7 +1815,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1844,7 +1835,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="4"/>
       <c r="C16" s="13" t="s">
@@ -1868,7 +1859,7 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>49</v>
       </c>
@@ -1908,16 +1899,16 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -1930,7 +1921,7 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="4"/>
       <c r="C19" s="9" t="s">
@@ -1954,7 +1945,7 @@
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1976,7 +1967,7 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2002,7 +1993,7 @@
       </c>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="4"/>
       <c r="C22" s="13"/>
@@ -2040,7 +2031,7 @@
       </c>
       <c r="T22" s="4"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>50</v>
       </c>
@@ -2102,29 +2093,29 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="4"/>
       <c r="C25" s="9" t="s">
@@ -2148,7 +2139,7 @@
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2160,7 +2151,7 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="13"/>
-      <c r="L27" s="17" t="s">
+      <c r="L27" s="16" t="s">
         <v>47</v>
       </c>
       <c r="M27" s="4"/>
@@ -2172,7 +2163,7 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="4"/>
       <c r="C28" s="13"/>
@@ -2182,18 +2173,18 @@
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="14" t="s">
         <v>14</v>
       </c>
       <c r="J28" s="4"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="25" t="s">
+      <c r="K28" s="20"/>
+      <c r="L28" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="23"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -2202,7 +2193,7 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>51</v>
       </c>
@@ -2233,7 +2224,7 @@
       <c r="J29" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="14" t="s">
+      <c r="K29" s="7" t="s">
         <v>10</v>
       </c>
       <c r="L29" s="7" t="s">
@@ -2256,29 +2247,29 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="4"/>
       <c r="C31" s="9" t="s">
@@ -2302,7 +2293,7 @@
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>92</v>
       </c>
@@ -2325,12 +2316,12 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -2338,7 +2329,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="4"/>
       <c r="C37" s="9" t="s">
@@ -2353,10 +2344,10 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="5"/>
       <c r="C40" s="4"/>
@@ -2369,7 +2360,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>52</v>
       </c>
@@ -2396,20 +2387,20 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="4"/>
       <c r="C43" s="9" t="s">
@@ -2424,9 +2415,9 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="21" t="s">
         <v>77</v>
       </c>
       <c r="C46" s="4"/>
@@ -2441,30 +2432,30 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="18" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="23" t="s">
+      <c r="B47" s="18"/>
+      <c r="C47" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="23" t="s">
+      <c r="G47" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="H47" s="23" t="s">
+      <c r="H47" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="I47" s="23" t="s">
+      <c r="I47" s="22" t="s">
         <v>64</v>
       </c>
       <c r="J47" s="4"/>
@@ -2472,22 +2463,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
       <c r="J48" s="4"/>
       <c r="K48" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="3:9">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="9" t="s">
         <v>1</v>
       </c>
@@ -2498,7 +2489,7 @@
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="3:9">
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -2515,20 +2506,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A5:C32"/>
   <sheetViews>
@@ -2536,12 +2527,12 @@
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2549,12 +2540,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>

</xml_diff>